<commit_message>
Added Screenshots of the Plots
</commit_message>
<xml_diff>
--- a/dsp_project/Data Collection/gpt_response_clean copy.xlsx
+++ b/dsp_project/Data Collection/gpt_response_clean copy.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasbrogaard/Documents/dsp_project/dsp_project/Data Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077993CE-C9C1-E848-AC26-3EB66E8EC78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5481800D-FBD7-7143-94F7-259195DA9AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Shitty prediction" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="483">
   <si>
     <t>Tingskovvej 70</t>
   </si>
@@ -2953,12 +2954,21 @@
   <si>
     <t>sqm</t>
   </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2972,6 +2982,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2981,7 +2998,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3004,14 +3021,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3317,8 +3365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18528,4 +18576,555 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FA1D95-CBAB-FA4D-9CFE-7C01A97DE7CC}">
+  <dimension ref="A1:Z30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <f>B2-E2</f>
+        <v>5260</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3003260</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2998000</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1970</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="5">
+        <v>3748</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5">
+        <v>72</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <f>B3-E3</f>
+        <v>-2886320</v>
+      </c>
+      <c r="B3" s="4">
+        <v>6108680</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8995000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1894</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4">
+        <v>4286</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="4">
+        <v>6</v>
+      </c>
+      <c r="L3" s="4">
+        <v>149</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="B6" s="6">
+        <f>B7-B8</f>
+        <v>5260</v>
+      </c>
+      <c r="C6" s="6">
+        <f>C7-C8</f>
+        <v>-2886320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="B7" s="6">
+        <v>3003260</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6108680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2998000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8995000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1970</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="B12" s="7">
+        <v>3748</v>
+      </c>
+      <c r="C12" s="6">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="B16" s="7">
+        <v>72</v>
+      </c>
+      <c r="C16" s="6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="B22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="B23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="B24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="B25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="B26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="B27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="B28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>